<commit_message>
start king and god
</commit_message>
<xml_diff>
--- a/wiktionary_pie.xlsx
+++ b/wiktionary_pie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\conlangs\pie-logographs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E6ECF9-3131-422C-AA59-33F29846888C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3E1FDB-734E-4F3C-B95F-F4072DC6FE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="6945" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20670" yWindow="7995" windowWidth="20370" windowHeight="9555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5426" uniqueCount="3996">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5435" uniqueCount="4001">
   <si>
     <t>headword</t>
   </si>
@@ -12011,6 +12011,21 @@
   </si>
   <si>
     <t>及</t>
+  </si>
+  <si>
+    <t>直</t>
+  </si>
+  <si>
+    <t>天</t>
+  </si>
+  <si>
+    <t>兒</t>
+  </si>
+  <si>
+    <t>子</t>
+  </si>
+  <si>
+    <t>心+毛？</t>
   </si>
 </sst>
 </file>
@@ -12386,8 +12401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A1251" workbookViewId="0">
+      <selection activeCell="C1265" sqref="C1265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13934,13 +13949,16 @@
       <c r="A92" t="s">
         <v>1299</v>
       </c>
+      <c r="B92" t="s">
+        <v>3998</v>
+      </c>
       <c r="C92" t="s">
         <v>1300</v>
       </c>
       <c r="D92" t="s">
         <v>430</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E92" s="2" t="s">
         <v>1301</v>
       </c>
     </row>
@@ -16236,7 +16254,7 @@
       <c r="D256" t="s">
         <v>430</v>
       </c>
-      <c r="E256" t="s">
+      <c r="E256" s="2" t="s">
         <v>737</v>
       </c>
     </row>
@@ -17157,6 +17175,9 @@
       <c r="A322" t="s">
         <v>2566</v>
       </c>
+      <c r="B322" t="s">
+        <v>3997</v>
+      </c>
       <c r="C322" t="s">
         <v>2567</v>
       </c>
@@ -22256,6 +22277,9 @@
       <c r="A686" t="s">
         <v>3489</v>
       </c>
+      <c r="B686" t="s">
+        <v>3996</v>
+      </c>
       <c r="C686" t="s">
         <v>3490</v>
       </c>
@@ -22270,6 +22294,9 @@
       <c r="A687" t="s">
         <v>1861</v>
       </c>
+      <c r="B687" t="s">
+        <v>3996</v>
+      </c>
       <c r="C687" t="s">
         <v>1862</v>
       </c>
@@ -22284,6 +22311,9 @@
       <c r="A688" t="s">
         <v>1320</v>
       </c>
+      <c r="B688" t="s">
+        <v>3996</v>
+      </c>
       <c r="C688" t="s">
         <v>1321</v>
       </c>
@@ -22298,13 +22328,16 @@
       <c r="A689" t="s">
         <v>960</v>
       </c>
+      <c r="B689" t="s">
+        <v>3996</v>
+      </c>
       <c r="C689" t="s">
         <v>961</v>
       </c>
       <c r="D689" t="s">
         <v>430</v>
       </c>
-      <c r="E689" t="s">
+      <c r="E689" s="2" t="s">
         <v>962</v>
       </c>
     </row>
@@ -22312,6 +22345,9 @@
       <c r="A690" t="s">
         <v>139</v>
       </c>
+      <c r="B690" t="s">
+        <v>3996</v>
+      </c>
       <c r="C690" t="s">
         <v>140</v>
       </c>
@@ -28682,6 +28718,9 @@
       <c r="A1145" t="s">
         <v>779</v>
       </c>
+      <c r="B1145" t="s">
+        <v>3999</v>
+      </c>
       <c r="C1145" t="s">
         <v>780</v>
       </c>
@@ -30304,7 +30343,7 @@
       <c r="D1260" t="s">
         <v>1132</v>
       </c>
-      <c r="E1260" t="s">
+      <c r="E1260" s="2" t="s">
         <v>2014</v>
       </c>
     </row>
@@ -30368,13 +30407,16 @@
       <c r="A1265" t="s">
         <v>2462</v>
       </c>
+      <c r="B1265" t="s">
+        <v>4000</v>
+      </c>
       <c r="C1265" t="s">
         <v>2463</v>
       </c>
       <c r="D1265" t="s">
         <v>1132</v>
       </c>
-      <c r="E1265" t="s">
+      <c r="E1265" s="2" t="s">
         <v>2464</v>
       </c>
     </row>
@@ -31397,6 +31439,11 @@
     <hyperlink ref="E13" r:id="rId41" xr:uid="{89F556BB-EA69-43AB-B565-DD6A8F25981C}"/>
     <hyperlink ref="E23" r:id="rId42" xr:uid="{C7ED0E7A-7C60-4C89-A84D-45D4BB4E6DD3}"/>
     <hyperlink ref="E85" r:id="rId43" xr:uid="{DB929ACA-C8F1-4CC2-9584-9C7C42697E20}"/>
+    <hyperlink ref="E689" r:id="rId44" xr:uid="{70EBA705-4DCE-4413-8E84-19953950FFDE}"/>
+    <hyperlink ref="E256" r:id="rId45" xr:uid="{DEAEC7E2-24F5-4023-88E3-32AB24982CCD}"/>
+    <hyperlink ref="E92" r:id="rId46" xr:uid="{54F093F0-2AEB-4486-83F5-5785F943A8FA}"/>
+    <hyperlink ref="E1260" r:id="rId47" xr:uid="{1464F93D-1CB7-46A2-BC92-53B34E37B47E}"/>
+    <hyperlink ref="E1265" r:id="rId48" xr:uid="{7237C2CB-4F04-432C-BB8B-26FF65E9F060}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>